<commit_message>
[RORO-4470][BT] corrected French apostrophe
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bentipper/Code/HMRC/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4680BD53-A0C6-2144-8BB8-FFC3F5A93C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DF3423-0AD0-6945-8174-1F3B1A335B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,9 +294,6 @@
     <t>Que se passe-t-il ensuite</t>
   </si>
   <si>
-    <t>Actuellement, vous n’avez pas besoin de vous soumettre à une inspection de vos marchandises. Vous devrez peut-être vous soumettre à d'autres contrôles lorsque vous vous rendrez en Irlande du Nord.</t>
-  </si>
-  <si>
     <t>Si vous terminez un mouvement de transit</t>
   </si>
   <si>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t>Možete nastaviti put od graničnog prijelaza dolaska do odredišta.</t>
+  </si>
+  <si>
+    <t>Actuellement, vous n’avez pas besoin de vous soumettre à une inspection de vos marchandises. Vous devrez peut-être vous soumettre à d’autres contrôles lorsque vous vous rendrez en Irlande du Nord.</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,13 +1130,13 @@
         <v>86</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N2" s="13"/>
     </row>
@@ -1172,13 +1172,13 @@
         <v>87</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N3" s="13"/>
     </row>
@@ -1214,13 +1214,13 @@
         <v>88</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N4" s="13"/>
     </row>
@@ -1253,16 +1253,16 @@
         <v>81</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N5" s="13"/>
     </row>
@@ -1295,16 +1295,16 @@
         <v>82</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N6" s="13"/>
     </row>
@@ -1337,16 +1337,16 @@
         <v>83</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N7" s="13"/>
     </row>
@@ -1379,20 +1379,20 @@
         <v>84</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="34" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
@@ -1421,16 +1421,16 @@
         <v>85</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N9" s="13"/>
     </row>

</xml_diff>

<commit_message>
[RORO-5257][SM]:  Clarify transit as border force transit
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6550B31-986B-6D4A-89DA-AA97A8762AB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512929D7-A0D9-FA4D-97A1-DA60FAC77101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="5980" windowWidth="30580" windowHeight="17720" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
+    <workbookView xWindow="4240" yWindow="760" windowWidth="30320" windowHeight="16000" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Translation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>KEY</t>
   </si>
@@ -72,131 +72,56 @@
     </r>
   </si>
   <si>
-    <t>Ask your haulier or importer to check the Import of products, animals, food and feed system (IPAFFS) to find out if you have any further inspections you need to attend.</t>
-  </si>
-  <si>
-    <t>For your DEFRA transit inspection</t>
-  </si>
-  <si>
-    <t>Speak to your haulier or importer to find out which Border Control Post (BCP) or other inspection location you need to attend on arrival.</t>
-  </si>
-  <si>
-    <t>Dotyczy Twojej kontroli tranzytowej przez Departament Środowiska, Żywności i Spraw Wiejskich (DEFRA)</t>
-  </si>
-  <si>
-    <t>Dowiedz się u swojego przewoźnika lub importera, do której placówki kontroli granicznej (BCP) lub innego punktu kontroli masz się zgłosić po przybyciu.</t>
-  </si>
-  <si>
-    <t>Poproś swojego przewoźnika lub importera o sprawdzenie w systemie importu produktów spożywczych, zwierząt, żywności i pasz (IPAFFS) czy musisz zgłosić się jeszcze na jakieś kontrole.</t>
-  </si>
-  <si>
-    <t>Pentru inspecția de tranzit DEFRA</t>
-  </si>
-  <si>
-    <t>Vorbiți cu transportatorul sau importatorul pentru a afla la ce Post de Control la Frontieră (BCP) sau altă locație de inspecție trebuie să mergeți la sosire.</t>
-  </si>
-  <si>
-    <t>Rugați transportatorul sau importatorul să verifice sistemul de import de produse, animale, alimente și furaje (IPAFFS) pentru a afla dacă sunt necesare alte inspecții suplimentare.</t>
-  </si>
-  <si>
-    <t>Dėl aplinkos, maisto ir kaimo reikalų departamento (DEFRA) vykdomos tranzito patikros</t>
-  </si>
-  <si>
-    <t>Paprašykite vežėjo arba importuotojo patikrinti produktų, gyvūnų, maisto ir pašarų importo sistemą (IPAFFS), kad sužinotumėte, ar turite praeiti dar kokias nors patikras.</t>
-  </si>
-  <si>
-    <t>Pasitarkite su vežėju arba importuotoju ir sužinokite, į kurį pasienio kontrolės postą (BCP) ar kitą tikrinimo vietą turite prisistatyti atvykę.</t>
-  </si>
-  <si>
-    <t>За вашата транзитна проверка от DEFRA</t>
-  </si>
-  <si>
-    <t>Говорете с вашия превозвач или вносител, за да разберете на кой граничен контролен пункт (ГКПП) или на кое друго място за проверка трябва да присъствате при пристигането.</t>
-  </si>
-  <si>
-    <t>Помолете вашия превозвач или вносител да провери Системата за внос на продукти, животни, храни и фуражи (IPAFFS), за да разберете дали има допълнителни проверки, на които трябва да присъствате.</t>
-  </si>
-  <si>
-    <t>Az Ön DEFRA-tranzitvizsgálatához</t>
-  </si>
-  <si>
-    <t>Beszéljen fuvarozójával vagy importőrével, hogy megtudja, melyik határállomáson (BCP) vagy más ellenőrzési helyen kell megjelennie érkezéskor.</t>
-  </si>
-  <si>
-    <t>Kérje meg fuvarozóját vagy importőrét, hogy ellenőrizze a Termékek, állatok, élelmiszerek és takarmányok behozatali rendszerét (IPAFFS), hogy megtudja, részt kell-e vennie további vizsgálatokon.</t>
-  </si>
-  <si>
-    <t>Para su inspección de tránsito DEFRA</t>
-  </si>
-  <si>
-    <t>Hable con su transportista o importador para saber a qué puesto de control fronterizo (BCP) o a qué otro lugar de inspección debe acudir a su llegada.</t>
-  </si>
-  <si>
-    <t>Pida a su transportista o importador que compruebe el sistema de importación de productos, animales, alimentos y piensos (IPAFFS) para saber si tiene que asistir a alguna inspección más.</t>
-  </si>
-  <si>
-    <t>Pour votre inspection de transit DEFRA (Département britannique de l’environnement, de l’alimentation et des affaires rurales)</t>
-  </si>
-  <si>
-    <t>Interrogez votre transporteur ou votre importateur pour savoir à quel poste de contrôle frontalier (BCP) ou à quel autre site d’inspection vous devez vous présenter à l’arrivée.</t>
-  </si>
-  <si>
-    <t>Demandez à votre transporteur ou à votre importateur de vérifier le système d’importation de produits, d’animaux, de denrées alimentaires et d’aliments pour animaux (IPAFFS) pour savoir si vous devez vous plier à d’autres inspections.</t>
-  </si>
-  <si>
-    <t>Promluvte si se svým dopravcem nebo dovozcem, chcete-li zjistit, která pracoviště přeshraniční kontroly (Border Control Post; BCP) nebo jiná kontrolní pracoviště musíte po příjezdu navštívit.</t>
-  </si>
-  <si>
-    <t>Za tranzitnu inspekciju DEFRA-e</t>
-  </si>
-  <si>
-    <t>Obratite se svojem prijevozniku ili uvozniku za informacije o tome na koju se graničnu kontrolnu postaju (BCP) ili drugo mjesto inspekcije morate javiti po dolasku.</t>
-  </si>
-  <si>
-    <t>Pitajte svojeg prijevoznika ili uvoznika da u sustavu za uvoz proizvoda, životinja, hrane i hrane za životinje (IPAFFS) provjeri morate li se javiti na dodatne inspekcije.</t>
-  </si>
-  <si>
-    <t>Für Ihre DEFRA Transit-Kontrolle</t>
-  </si>
-  <si>
-    <t>Wenden Sie sich an Ihren Spediteur oder Importeur, um herauszufinden, welche Grenzkontrollstelle (BCP) oder sonstige Kontrollstelle Sie bei Ihrer Ankunft aufsuchen müssen.</t>
-  </si>
-  <si>
-    <t>Bitten Sie Ihren Spediteur oder Importeur, im System zur Einfuhr von Erzeugnissen, Tieren, Lebens- und Futtermitteln (IPAFFS) herauszufinden,  ob für Sie noch weitere Kontrollen notwendig sind.</t>
-  </si>
-  <si>
-    <t>inspection_needed.defra_transit.heading</t>
-  </si>
-  <si>
-    <t>inspection_needed_import.what_next.bcp_content</t>
-  </si>
-  <si>
-    <t>inspection_needed.defra_transit.ipaffs</t>
+    <t>For your Border Force transit inspection</t>
+  </si>
+  <si>
+    <t>Dotyczy Twojej kontroli tranzytowej przez straż graniczną</t>
+  </si>
+  <si>
+    <t>Pentru inspecția de tranzit a Poliției de Frontieră</t>
+  </si>
+  <si>
+    <t>Dėl tranzito patikros pasienio apsaugos tarnyboje</t>
+  </si>
+  <si>
+    <t>За вашата транзитна проверка от граничните служби</t>
+  </si>
+  <si>
+    <t>Az Ön Border Force-tranzitvizsgálatához</t>
+  </si>
+  <si>
+    <t>Para su inspección de tránsito por la guardia fronteriza</t>
+  </si>
+  <si>
+    <t>Pour votre inspection de transit Border Force (agence britannique de contrôle frontalier)</t>
+  </si>
+  <si>
+    <t>Pro vaši tranzitní prohlídku pohraničními jednotkami</t>
+  </si>
+  <si>
+    <t>Za tranzitnu inspekciju granične policije</t>
+  </si>
+  <si>
+    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (UKBF)</t>
   </si>
   <si>
     <t>Welsh</t>
   </si>
   <si>
-    <t>O ran eich archwiliad cludo gan DEFRA</t>
-  </si>
-  <si>
-    <t>Siaradwch â’ch cludwr neu fewnforiwr i gael gwybod pa Fan Rheoli Wrth y Ffin (BCP) neu leoliad archwilio arall sydd angen i chi ei fynychu wrth gyrraedd.</t>
-  </si>
-  <si>
-    <t>Gofynnwch i’ch cludwr neu fewnforiwr i wirio’r system mewnforio cynhyrchion, anifeiliaid, bwyd a bwyd anifeiliaid i gael gwybod a oes angen i chi fynychu unrhyw archwiliadau pellach.</t>
-  </si>
-  <si>
-    <t>K tranzitní prohlídce DEFRA</t>
-  </si>
-  <si>
-    <t>Požádejte dopravce nebo dovozce, aby zkontroloval systém IPAFFS pro dovoz výrobků, zvířat, potravin a krmiv, chcete-li zjistit, zda se musíte zúčastnit jakýchkoli dalších prohlídek.</t>
+    <t>O ran eich archwiliad cludo gan Lu’r Ffiniau</t>
+  </si>
+  <si>
+    <t>inspection_needed_import.bf_transit.heading</t>
+  </si>
+  <si>
+    <t>inspection_needed_export.bf_transit.heading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,11 +177,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -283,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -367,28 +287,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -417,22 +322,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -751,27 +647,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.6640625" style="7" customWidth="1"/>
     <col min="2" max="2" width="66.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="10" customWidth="1"/>
     <col min="4" max="7" width="15.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="15.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="89.83203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="89.83203125" style="10" customWidth="1"/>
     <col min="14" max="16384" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -809,136 +705,93 @@
         <v>10</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="113" thickBot="1">
+    <row r="2" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="F2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="I2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="M2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" ht="209" thickBot="1">
+    <row r="3" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="G3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>38</v>
+      <c r="J3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="225" thickBot="1">
-      <c r="A4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="19">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="M5" s="9"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M4" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
[RORO-5094][SM]: Defra transit hold content (#22)
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A94E7A2-4BC4-1642-98AC-DDC7F99B93F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6550B31-986B-6D4A-89DA-AA97A8762AB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="780" windowWidth="34140" windowHeight="20100" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
+    <workbookView xWindow="2180" yWindow="5980" windowWidth="30580" windowHeight="17720" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Translation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+  <si>
+    <t>KEY</t>
+  </si>
   <si>
     <t>English</t>
   </si>
@@ -69,58 +72,140 @@
     </r>
   </si>
   <si>
-    <t>Key</t>
+    <t>Ask your haulier or importer to check the Import of products, animals, food and feed system (IPAFFS) to find out if you have any further inspections you need to attend.</t>
+  </si>
+  <si>
+    <t>For your DEFRA transit inspection</t>
+  </si>
+  <si>
+    <t>Speak to your haulier or importer to find out which Border Control Post (BCP) or other inspection location you need to attend on arrival.</t>
+  </si>
+  <si>
+    <t>Dotyczy Twojej kontroli tranzytowej przez Departament Środowiska, Żywności i Spraw Wiejskich (DEFRA)</t>
+  </si>
+  <si>
+    <t>Dowiedz się u swojego przewoźnika lub importera, do której placówki kontroli granicznej (BCP) lub innego punktu kontroli masz się zgłosić po przybyciu.</t>
+  </si>
+  <si>
+    <t>Poproś swojego przewoźnika lub importera o sprawdzenie w systemie importu produktów spożywczych, zwierząt, żywności i pasz (IPAFFS) czy musisz zgłosić się jeszcze na jakieś kontrole.</t>
+  </si>
+  <si>
+    <t>Pentru inspecția de tranzit DEFRA</t>
+  </si>
+  <si>
+    <t>Vorbiți cu transportatorul sau importatorul pentru a afla la ce Post de Control la Frontieră (BCP) sau altă locație de inspecție trebuie să mergeți la sosire.</t>
+  </si>
+  <si>
+    <t>Rugați transportatorul sau importatorul să verifice sistemul de import de produse, animale, alimente și furaje (IPAFFS) pentru a afla dacă sunt necesare alte inspecții suplimentare.</t>
+  </si>
+  <si>
+    <t>Dėl aplinkos, maisto ir kaimo reikalų departamento (DEFRA) vykdomos tranzito patikros</t>
+  </si>
+  <si>
+    <t>Paprašykite vežėjo arba importuotojo patikrinti produktų, gyvūnų, maisto ir pašarų importo sistemą (IPAFFS), kad sužinotumėte, ar turite praeiti dar kokias nors patikras.</t>
+  </si>
+  <si>
+    <t>Pasitarkite su vežėju arba importuotoju ir sužinokite, į kurį pasienio kontrolės postą (BCP) ar kitą tikrinimo vietą turite prisistatyti atvykę.</t>
+  </si>
+  <si>
+    <t>За вашата транзитна проверка от DEFRA</t>
+  </si>
+  <si>
+    <t>Говорете с вашия превозвач или вносител, за да разберете на кой граничен контролен пункт (ГКПП) или на кое друго място за проверка трябва да присъствате при пристигането.</t>
+  </si>
+  <si>
+    <t>Помолете вашия превозвач или вносител да провери Системата за внос на продукти, животни, храни и фуражи (IPAFFS), за да разберете дали има допълнителни проверки, на които трябва да присъствате.</t>
+  </si>
+  <si>
+    <t>Az Ön DEFRA-tranzitvizsgálatához</t>
+  </si>
+  <si>
+    <t>Beszéljen fuvarozójával vagy importőrével, hogy megtudja, melyik határállomáson (BCP) vagy más ellenőrzési helyen kell megjelennie érkezéskor.</t>
+  </si>
+  <si>
+    <t>Kérje meg fuvarozóját vagy importőrét, hogy ellenőrizze a Termékek, állatok, élelmiszerek és takarmányok behozatali rendszerét (IPAFFS), hogy megtudja, részt kell-e vennie további vizsgálatokon.</t>
+  </si>
+  <si>
+    <t>Para su inspección de tránsito DEFRA</t>
+  </si>
+  <si>
+    <t>Hable con su transportista o importador para saber a qué puesto de control fronterizo (BCP) o a qué otro lugar de inspección debe acudir a su llegada.</t>
+  </si>
+  <si>
+    <t>Pida a su transportista o importador que compruebe el sistema de importación de productos, animales, alimentos y piensos (IPAFFS) para saber si tiene que asistir a alguna inspección más.</t>
+  </si>
+  <si>
+    <t>Pour votre inspection de transit DEFRA (Département britannique de l’environnement, de l’alimentation et des affaires rurales)</t>
+  </si>
+  <si>
+    <t>Interrogez votre transporteur ou votre importateur pour savoir à quel poste de contrôle frontalier (BCP) ou à quel autre site d’inspection vous devez vous présenter à l’arrivée.</t>
+  </si>
+  <si>
+    <t>Demandez à votre transporteur ou à votre importateur de vérifier le système d’importation de produits, d’animaux, de denrées alimentaires et d’aliments pour animaux (IPAFFS) pour savoir si vous devez vous plier à d’autres inspections.</t>
+  </si>
+  <si>
+    <t>Promluvte si se svým dopravcem nebo dovozcem, chcete-li zjistit, která pracoviště přeshraniční kontroly (Border Control Post; BCP) nebo jiná kontrolní pracoviště musíte po příjezdu navštívit.</t>
+  </si>
+  <si>
+    <t>Za tranzitnu inspekciju DEFRA-e</t>
+  </si>
+  <si>
+    <t>Obratite se svojem prijevozniku ili uvozniku za informacije o tome na koju se graničnu kontrolnu postaju (BCP) ili drugo mjesto inspekcije morate javiti po dolasku.</t>
+  </si>
+  <si>
+    <t>Pitajte svojeg prijevoznika ili uvoznika da u sustavu za uvoz proizvoda, životinja, hrane i hrane za životinje (IPAFFS) provjeri morate li se javiti na dodatne inspekcije.</t>
+  </si>
+  <si>
+    <t>Für Ihre DEFRA Transit-Kontrolle</t>
+  </si>
+  <si>
+    <t>Wenden Sie sich an Ihren Spediteur oder Importeur, um herauszufinden, welche Grenzkontrollstelle (BCP) oder sonstige Kontrollstelle Sie bei Ihrer Ankunft aufsuchen müssen.</t>
+  </si>
+  <si>
+    <t>Bitten Sie Ihren Spediteur oder Importeur, im System zur Einfuhr von Erzeugnissen, Tieren, Lebens- und Futtermitteln (IPAFFS) herauszufinden,  ob für Sie noch weitere Kontrollen notwendig sind.</t>
+  </si>
+  <si>
+    <t>inspection_needed.defra_transit.heading</t>
+  </si>
+  <si>
+    <t>inspection_needed_import.what_next.bcp_content</t>
+  </si>
+  <si>
+    <t>inspection_needed.defra_transit.ipaffs</t>
   </si>
   <si>
     <t>Welsh</t>
   </si>
   <si>
-    <t>For your ENS (Safety and Security) inspection</t>
-  </si>
-  <si>
-    <t>Do kontroli Twojej przywozowej deklaracji skróconej (bezpieczeństwo i ochrona) [ENS (Safety and Security)]</t>
-  </si>
-  <si>
-    <t>Pentru inspecția dumneavoastră ENS (siguranță și securitate)</t>
-  </si>
-  <si>
-    <t>Jūsų ENS (saugos ir saugumo) patikrai</t>
-  </si>
-  <si>
-    <t>За проверка на декларация за внос ENS (безопасност и сигурност)</t>
-  </si>
-  <si>
-    <t>Az Ön ENS- (biztonsági és védelmi) ellenőrzéséhez</t>
-  </si>
-  <si>
-    <t>Para la inspección de su declaración ENS (Seguridad y Protección)</t>
-  </si>
-  <si>
-    <t>Pour votre inspection ENS (Sûreté et Sécurité)</t>
-  </si>
-  <si>
-    <t>Für Ihre ENS-Eingangsanmeldungs-Kontrolle (Sicherheit und Gefahrenabwehr)</t>
-  </si>
-  <si>
-    <t>Pro vaši kontrolu vstupního souhrnného prohlášení (ENS)</t>
-  </si>
-  <si>
-    <t>Za provjeru vaše ENS deklaracije (deklaracije o sigurnosti i zaštiti)</t>
-  </si>
-  <si>
-    <t>inspection_needed_import.sns.heading</t>
-  </si>
-  <si>
-    <t>Ar gyfer eich archwiliad ENS (Diogelwch)</t>
+    <t>O ran eich archwiliad cludo gan DEFRA</t>
+  </si>
+  <si>
+    <t>Siaradwch â’ch cludwr neu fewnforiwr i gael gwybod pa Fan Rheoli Wrth y Ffin (BCP) neu leoliad archwilio arall sydd angen i chi ei fynychu wrth gyrraedd.</t>
+  </si>
+  <si>
+    <t>Gofynnwch i’ch cludwr neu fewnforiwr i wirio’r system mewnforio cynhyrchion, anifeiliaid, bwyd a bwyd anifeiliaid i gael gwybod a oes angen i chi fynychu unrhyw archwiliadau pellach.</t>
+  </si>
+  <si>
+    <t>K tranzitní prohlídce DEFRA</t>
+  </si>
+  <si>
+    <t>Požádejte dopravce nebo dovozce, aby zkontroloval systém IPAFFS pro dovoz výrobků, zvířat, potravin a krmiv, chcete-li zjistit, zda se musíte zúčastnit jakýchkoli dalších prohlídek.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,13 +239,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -168,6 +246,18 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,12 +283,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -211,9 +316,7 @@
       <top style="thin">
         <color rgb="FFCACACA"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFCACACA"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -224,22 +327,7 @@
       <top style="thin">
         <color rgb="FFCACACA"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFCACACA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFCACACA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCACACA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCACACA"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -252,8 +340,30 @@
       <top style="thin">
         <color theme="2"/>
       </top>
-      <bottom style="thin">
-        <color theme="2"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCACACA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCACACA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -264,23 +374,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -288,47 +385,61 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{737C23FE-2062-7949-9733-88E9960A1E96}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{02148EF0-8DBA-A540-BA5A-717DFE220657}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{145767DE-5E71-4FDD-AAB0-DFA3AC73381F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,114 +753,195 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="40.5" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="72.83203125" style="6" customWidth="1"/>
-    <col min="5" max="7" width="15.33203125" style="6" customWidth="1"/>
-    <col min="8" max="12" width="15.33203125" style="7" customWidth="1"/>
-    <col min="13" max="13" width="89.83203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="66.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="11" customWidth="1"/>
+    <col min="4" max="7" width="15.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="89.83203125" style="11" customWidth="1"/>
+    <col min="14" max="16384" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="18" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="113" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="209" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="225" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="C4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="103" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M3" s="11"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M5" s="11"/>
+    <row r="5" spans="1:13" ht="19">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10"/>
+      <c r="M5" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[RORO-5257][SM]: Clarify transit as border force transit (#23)
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6550B31-986B-6D4A-89DA-AA97A8762AB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512929D7-A0D9-FA4D-97A1-DA60FAC77101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="5980" windowWidth="30580" windowHeight="17720" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
+    <workbookView xWindow="4240" yWindow="760" windowWidth="30320" windowHeight="16000" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Translation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>KEY</t>
   </si>
@@ -72,131 +72,56 @@
     </r>
   </si>
   <si>
-    <t>Ask your haulier or importer to check the Import of products, animals, food and feed system (IPAFFS) to find out if you have any further inspections you need to attend.</t>
-  </si>
-  <si>
-    <t>For your DEFRA transit inspection</t>
-  </si>
-  <si>
-    <t>Speak to your haulier or importer to find out which Border Control Post (BCP) or other inspection location you need to attend on arrival.</t>
-  </si>
-  <si>
-    <t>Dotyczy Twojej kontroli tranzytowej przez Departament Środowiska, Żywności i Spraw Wiejskich (DEFRA)</t>
-  </si>
-  <si>
-    <t>Dowiedz się u swojego przewoźnika lub importera, do której placówki kontroli granicznej (BCP) lub innego punktu kontroli masz się zgłosić po przybyciu.</t>
-  </si>
-  <si>
-    <t>Poproś swojego przewoźnika lub importera o sprawdzenie w systemie importu produktów spożywczych, zwierząt, żywności i pasz (IPAFFS) czy musisz zgłosić się jeszcze na jakieś kontrole.</t>
-  </si>
-  <si>
-    <t>Pentru inspecția de tranzit DEFRA</t>
-  </si>
-  <si>
-    <t>Vorbiți cu transportatorul sau importatorul pentru a afla la ce Post de Control la Frontieră (BCP) sau altă locație de inspecție trebuie să mergeți la sosire.</t>
-  </si>
-  <si>
-    <t>Rugați transportatorul sau importatorul să verifice sistemul de import de produse, animale, alimente și furaje (IPAFFS) pentru a afla dacă sunt necesare alte inspecții suplimentare.</t>
-  </si>
-  <si>
-    <t>Dėl aplinkos, maisto ir kaimo reikalų departamento (DEFRA) vykdomos tranzito patikros</t>
-  </si>
-  <si>
-    <t>Paprašykite vežėjo arba importuotojo patikrinti produktų, gyvūnų, maisto ir pašarų importo sistemą (IPAFFS), kad sužinotumėte, ar turite praeiti dar kokias nors patikras.</t>
-  </si>
-  <si>
-    <t>Pasitarkite su vežėju arba importuotoju ir sužinokite, į kurį pasienio kontrolės postą (BCP) ar kitą tikrinimo vietą turite prisistatyti atvykę.</t>
-  </si>
-  <si>
-    <t>За вашата транзитна проверка от DEFRA</t>
-  </si>
-  <si>
-    <t>Говорете с вашия превозвач или вносител, за да разберете на кой граничен контролен пункт (ГКПП) или на кое друго място за проверка трябва да присъствате при пристигането.</t>
-  </si>
-  <si>
-    <t>Помолете вашия превозвач или вносител да провери Системата за внос на продукти, животни, храни и фуражи (IPAFFS), за да разберете дали има допълнителни проверки, на които трябва да присъствате.</t>
-  </si>
-  <si>
-    <t>Az Ön DEFRA-tranzitvizsgálatához</t>
-  </si>
-  <si>
-    <t>Beszéljen fuvarozójával vagy importőrével, hogy megtudja, melyik határállomáson (BCP) vagy más ellenőrzési helyen kell megjelennie érkezéskor.</t>
-  </si>
-  <si>
-    <t>Kérje meg fuvarozóját vagy importőrét, hogy ellenőrizze a Termékek, állatok, élelmiszerek és takarmányok behozatali rendszerét (IPAFFS), hogy megtudja, részt kell-e vennie további vizsgálatokon.</t>
-  </si>
-  <si>
-    <t>Para su inspección de tránsito DEFRA</t>
-  </si>
-  <si>
-    <t>Hable con su transportista o importador para saber a qué puesto de control fronterizo (BCP) o a qué otro lugar de inspección debe acudir a su llegada.</t>
-  </si>
-  <si>
-    <t>Pida a su transportista o importador que compruebe el sistema de importación de productos, animales, alimentos y piensos (IPAFFS) para saber si tiene que asistir a alguna inspección más.</t>
-  </si>
-  <si>
-    <t>Pour votre inspection de transit DEFRA (Département britannique de l’environnement, de l’alimentation et des affaires rurales)</t>
-  </si>
-  <si>
-    <t>Interrogez votre transporteur ou votre importateur pour savoir à quel poste de contrôle frontalier (BCP) ou à quel autre site d’inspection vous devez vous présenter à l’arrivée.</t>
-  </si>
-  <si>
-    <t>Demandez à votre transporteur ou à votre importateur de vérifier le système d’importation de produits, d’animaux, de denrées alimentaires et d’aliments pour animaux (IPAFFS) pour savoir si vous devez vous plier à d’autres inspections.</t>
-  </si>
-  <si>
-    <t>Promluvte si se svým dopravcem nebo dovozcem, chcete-li zjistit, která pracoviště přeshraniční kontroly (Border Control Post; BCP) nebo jiná kontrolní pracoviště musíte po příjezdu navštívit.</t>
-  </si>
-  <si>
-    <t>Za tranzitnu inspekciju DEFRA-e</t>
-  </si>
-  <si>
-    <t>Obratite se svojem prijevozniku ili uvozniku za informacije o tome na koju se graničnu kontrolnu postaju (BCP) ili drugo mjesto inspekcije morate javiti po dolasku.</t>
-  </si>
-  <si>
-    <t>Pitajte svojeg prijevoznika ili uvoznika da u sustavu za uvoz proizvoda, životinja, hrane i hrane za životinje (IPAFFS) provjeri morate li se javiti na dodatne inspekcije.</t>
-  </si>
-  <si>
-    <t>Für Ihre DEFRA Transit-Kontrolle</t>
-  </si>
-  <si>
-    <t>Wenden Sie sich an Ihren Spediteur oder Importeur, um herauszufinden, welche Grenzkontrollstelle (BCP) oder sonstige Kontrollstelle Sie bei Ihrer Ankunft aufsuchen müssen.</t>
-  </si>
-  <si>
-    <t>Bitten Sie Ihren Spediteur oder Importeur, im System zur Einfuhr von Erzeugnissen, Tieren, Lebens- und Futtermitteln (IPAFFS) herauszufinden,  ob für Sie noch weitere Kontrollen notwendig sind.</t>
-  </si>
-  <si>
-    <t>inspection_needed.defra_transit.heading</t>
-  </si>
-  <si>
-    <t>inspection_needed_import.what_next.bcp_content</t>
-  </si>
-  <si>
-    <t>inspection_needed.defra_transit.ipaffs</t>
+    <t>For your Border Force transit inspection</t>
+  </si>
+  <si>
+    <t>Dotyczy Twojej kontroli tranzytowej przez straż graniczną</t>
+  </si>
+  <si>
+    <t>Pentru inspecția de tranzit a Poliției de Frontieră</t>
+  </si>
+  <si>
+    <t>Dėl tranzito patikros pasienio apsaugos tarnyboje</t>
+  </si>
+  <si>
+    <t>За вашата транзитна проверка от граничните служби</t>
+  </si>
+  <si>
+    <t>Az Ön Border Force-tranzitvizsgálatához</t>
+  </si>
+  <si>
+    <t>Para su inspección de tránsito por la guardia fronteriza</t>
+  </si>
+  <si>
+    <t>Pour votre inspection de transit Border Force (agence britannique de contrôle frontalier)</t>
+  </si>
+  <si>
+    <t>Pro vaši tranzitní prohlídku pohraničními jednotkami</t>
+  </si>
+  <si>
+    <t>Za tranzitnu inspekciju granične policije</t>
+  </si>
+  <si>
+    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (UKBF)</t>
   </si>
   <si>
     <t>Welsh</t>
   </si>
   <si>
-    <t>O ran eich archwiliad cludo gan DEFRA</t>
-  </si>
-  <si>
-    <t>Siaradwch â’ch cludwr neu fewnforiwr i gael gwybod pa Fan Rheoli Wrth y Ffin (BCP) neu leoliad archwilio arall sydd angen i chi ei fynychu wrth gyrraedd.</t>
-  </si>
-  <si>
-    <t>Gofynnwch i’ch cludwr neu fewnforiwr i wirio’r system mewnforio cynhyrchion, anifeiliaid, bwyd a bwyd anifeiliaid i gael gwybod a oes angen i chi fynychu unrhyw archwiliadau pellach.</t>
-  </si>
-  <si>
-    <t>K tranzitní prohlídce DEFRA</t>
-  </si>
-  <si>
-    <t>Požádejte dopravce nebo dovozce, aby zkontroloval systém IPAFFS pro dovoz výrobků, zvířat, potravin a krmiv, chcete-li zjistit, zda se musíte zúčastnit jakýchkoli dalších prohlídek.</t>
+    <t>O ran eich archwiliad cludo gan Lu’r Ffiniau</t>
+  </si>
+  <si>
+    <t>inspection_needed_import.bf_transit.heading</t>
+  </si>
+  <si>
+    <t>inspection_needed_export.bf_transit.heading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,11 +177,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -283,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -367,28 +287,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -417,22 +322,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -751,27 +647,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.6640625" style="7" customWidth="1"/>
     <col min="2" max="2" width="66.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="10" customWidth="1"/>
     <col min="4" max="7" width="15.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="15.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="89.83203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="89.83203125" style="10" customWidth="1"/>
     <col min="14" max="16384" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -809,136 +705,93 @@
         <v>10</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="113" thickBot="1">
+    <row r="2" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="F2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="I2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="M2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" ht="209" thickBot="1">
+    <row r="3" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="G3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>38</v>
+      <c r="J3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="225" thickBot="1">
-      <c r="A4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="19">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="M5" s="9"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M4" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
[RORO-5257][SM]: Updated German translation for bf_transit
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512929D7-A0D9-FA4D-97A1-DA60FAC77101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E40672E-89A0-2141-9A1F-4298C774E8DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="760" windowWidth="30320" windowHeight="16000" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
   </bookViews>
@@ -25,90 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>KEY</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Romanian</t>
-  </si>
-  <si>
-    <t>Lithuanian</t>
-  </si>
-  <si>
-    <t>Bulgarian</t>
-  </si>
-  <si>
-    <t>Hungarian</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
     <t>German</t>
-  </si>
-  <si>
-    <t>Czech</t>
-  </si>
-  <si>
-    <t>Croatian</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Polish</t>
-    </r>
-  </si>
-  <si>
-    <t>For your Border Force transit inspection</t>
-  </si>
-  <si>
-    <t>Dotyczy Twojej kontroli tranzytowej przez straż graniczną</t>
-  </si>
-  <si>
-    <t>Pentru inspecția de tranzit a Poliției de Frontieră</t>
-  </si>
-  <si>
-    <t>Dėl tranzito patikros pasienio apsaugos tarnyboje</t>
-  </si>
-  <si>
-    <t>За вашата транзитна проверка от граничните служби</t>
-  </si>
-  <si>
-    <t>Az Ön Border Force-tranzitvizsgálatához</t>
-  </si>
-  <si>
-    <t>Para su inspección de tránsito por la guardia fronteriza</t>
-  </si>
-  <si>
-    <t>Pour votre inspection de transit Border Force (agence britannique de contrôle frontalier)</t>
-  </si>
-  <si>
-    <t>Pro vaši tranzitní prohlídku pohraničními jednotkami</t>
-  </si>
-  <si>
-    <t>Za tranzitnu inspekciju granične policije</t>
-  </si>
-  <si>
-    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (UKBF)</t>
-  </si>
-  <si>
-    <t>Welsh</t>
-  </si>
-  <si>
-    <t>O ran eich archwiliad cludo gan Lu’r Ffiniau</t>
   </si>
   <si>
     <t>inspection_needed_import.bf_transit.heading</t>
@@ -116,21 +38,17 @@
   <si>
     <t>inspection_needed_export.bf_transit.heading</t>
   </si>
+  <si>
+    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (Border Force)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -183,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,14 +114,8 @@
         <bgColor rgb="FFBDBDBD"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -240,30 +152,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFCACACA"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCACACA"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FFCACACA"/>
@@ -290,33 +178,24 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -325,10 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,154 +523,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="66.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="10" customWidth="1"/>
-    <col min="4" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="89.83203125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="11" style="7"/>
+    <col min="1" max="1" width="72.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="89.83203125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M4" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[RORO-5257][SM]: Updated German translation for bf_transit (#24)
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512929D7-A0D9-FA4D-97A1-DA60FAC77101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E40672E-89A0-2141-9A1F-4298C774E8DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="760" windowWidth="30320" windowHeight="16000" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
   </bookViews>
@@ -25,90 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>KEY</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Romanian</t>
-  </si>
-  <si>
-    <t>Lithuanian</t>
-  </si>
-  <si>
-    <t>Bulgarian</t>
-  </si>
-  <si>
-    <t>Hungarian</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
     <t>German</t>
-  </si>
-  <si>
-    <t>Czech</t>
-  </si>
-  <si>
-    <t>Croatian</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Polish</t>
-    </r>
-  </si>
-  <si>
-    <t>For your Border Force transit inspection</t>
-  </si>
-  <si>
-    <t>Dotyczy Twojej kontroli tranzytowej przez straż graniczną</t>
-  </si>
-  <si>
-    <t>Pentru inspecția de tranzit a Poliției de Frontieră</t>
-  </si>
-  <si>
-    <t>Dėl tranzito patikros pasienio apsaugos tarnyboje</t>
-  </si>
-  <si>
-    <t>За вашата транзитна проверка от граничните служби</t>
-  </si>
-  <si>
-    <t>Az Ön Border Force-tranzitvizsgálatához</t>
-  </si>
-  <si>
-    <t>Para su inspección de tránsito por la guardia fronteriza</t>
-  </si>
-  <si>
-    <t>Pour votre inspection de transit Border Force (agence britannique de contrôle frontalier)</t>
-  </si>
-  <si>
-    <t>Pro vaši tranzitní prohlídku pohraničními jednotkami</t>
-  </si>
-  <si>
-    <t>Za tranzitnu inspekciju granične policije</t>
-  </si>
-  <si>
-    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (UKBF)</t>
-  </si>
-  <si>
-    <t>Welsh</t>
-  </si>
-  <si>
-    <t>O ran eich archwiliad cludo gan Lu’r Ffiniau</t>
   </si>
   <si>
     <t>inspection_needed_import.bf_transit.heading</t>
@@ -116,21 +38,17 @@
   <si>
     <t>inspection_needed_export.bf_transit.heading</t>
   </si>
+  <si>
+    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (Border Force)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -183,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,14 +114,8 @@
         <bgColor rgb="FFBDBDBD"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -240,30 +152,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFCACACA"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCACACA"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FFCACACA"/>
@@ -290,33 +178,24 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -325,10 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,154 +523,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="66.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="10" customWidth="1"/>
-    <col min="4" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="89.83203125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="11" style="7"/>
+    <col min="1" max="1" width="72.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="89.83203125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M4" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[RORO-5500][SM]: start page content changes
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E40672E-89A0-2141-9A1F-4298C774E8DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DEC501-569A-104E-9337-B747B7228791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="760" windowWidth="30320" windowHeight="16000" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
+    <workbookView xWindow="3020" yWindow="1240" windowWidth="30240" windowHeight="17360" xr2:uid="{BB80C880-331F-46F2-AF17-7FB10C103EC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Translation" sheetId="1" r:id="rId1"/>
+    <sheet name="Translation" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,28 +25,98 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Lithuanian</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Croatian</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>If the movement needs an inspection</t>
+  </si>
+  <si>
+    <t>Pokud je potřeba provést kontrolu pohybu</t>
+  </si>
+  <si>
+    <t>Ako kretanje mora proći inspekciju</t>
+  </si>
+  <si>
+    <t>Dacă este necesară o inspecție pentru transport</t>
+  </si>
+  <si>
+    <t>Jei gabenamą krovinį reikia patikrinti</t>
+  </si>
+  <si>
+    <t>Ако има нужда от проверка на движението</t>
+  </si>
+  <si>
+    <t>Ha az árumozgatást ellenőrizni kell</t>
+  </si>
+  <si>
+    <t>Jeżeli przemieszczenie wymaga kontroli</t>
+  </si>
+  <si>
+    <t>Si el tránsito necesita inspección</t>
+  </si>
+  <si>
+    <t>Si le mouvement nécessite une inspection</t>
+  </si>
+  <si>
+    <t>Wenn für die Warenbeförderung eine Kontrolle erforderlich ist</t>
+  </si>
+  <si>
+    <t>Welsh</t>
+  </si>
+  <si>
+    <t>Os oes angen i’r symudiad hwn gael ei archwilio</t>
+  </si>
+  <si>
+    <t>start_page.before_you_start.inspection_needed</t>
+  </si>
   <si>
     <t>KEY</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>inspection_needed_import.bf_transit.heading</t>
-  </si>
-  <si>
-    <t>inspection_needed_export.bf_transit.heading</t>
-  </si>
-  <si>
-    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (Border Force)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,47 +131,47 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helevetica"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +184,12 @@
         <bgColor rgb="FFBDBDBD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -121,21 +197,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -152,6 +213,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFCACACA"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCACACA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFCACACA"/>
@@ -162,56 +247,42 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{737C23FE-2062-7949-9733-88E9960A1E96}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{145767DE-5E71-4FDD-AAB0-DFA3AC73381F}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{0379D854-FC25-4F16-93FD-6B38214E7791}"/>
+    <cellStyle name="Normál 2" xfId="3" xr:uid="{66BDFD21-A3E8-4147-B676-F9F30F3B4BD9}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{2D952BDF-2BA3-48EA-9E89-B93B515F91F4}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,50 +593,424 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88F8323-D81A-7742-91D0-E5D4A31A9FBE}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="72.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="89.83203125" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="4"/>
+    <col min="1" max="1" width="43" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100" style="1" customWidth="1"/>
+    <col min="4" max="4" width="89.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="114.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="74.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="119.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="78.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="102" style="1" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="120.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="80.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="95" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
+    <row r="2" spans="1:13" ht="22">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:13">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="10"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D23464B46C9A6C438A9A63FA525492B5" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="816d63d098657adee5e1780dd4373ff3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78648aa0-189c-4913-b480-8f083842eefa" xmlns:ns3="252b28bd-d93f-4b99-825e-07b76ab2fd6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc6b77c161da750edc5730dfe65423ec" ns2:_="" ns3:_="">
+    <xsd:import namespace="78648aa0-189c-4913-b480-8f083842eefa"/>
+    <xsd:import namespace="252b28bd-d93f-4b99-825e-07b76ab2fd6b"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="78648aa0-189c-4913-b480-8f083842eefa" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a3ebb39f-d69b-4575-80f5-9912993956e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="252b28bd-d93f-4b99-825e-07b76ab2fd6b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f7f7e37a-fab3-43f2-9f32-1e0449a57439}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="252b28bd-d93f-4b99-825e-07b76ab2fd6b">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B41EF1-37C1-4B99-A8DD-7B54478B18A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4460EA2-5BBD-4FA9-A1BE-350942C106E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="78648aa0-189c-4913-b480-8f083842eefa"/>
+    <ds:schemaRef ds:uri="252b28bd-d93f-4b99-825e-07b76ab2fd6b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[RORO-5500][SM]: start page content changes (#31)
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh/hmrc/driver-inspection-notification-frontend/test-resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E40672E-89A0-2141-9A1F-4298C774E8DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DEC501-569A-104E-9337-B747B7228791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="760" windowWidth="30320" windowHeight="16000" xr2:uid="{49873166-AB72-9444-9FF4-478626AA29B4}"/>
+    <workbookView xWindow="3020" yWindow="1240" windowWidth="30240" windowHeight="17360" xr2:uid="{BB80C880-331F-46F2-AF17-7FB10C103EC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Translation" sheetId="1" r:id="rId1"/>
+    <sheet name="Translation" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,28 +25,98 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Lithuanian</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Croatian</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>If the movement needs an inspection</t>
+  </si>
+  <si>
+    <t>Pokud je potřeba provést kontrolu pohybu</t>
+  </si>
+  <si>
+    <t>Ako kretanje mora proći inspekciju</t>
+  </si>
+  <si>
+    <t>Dacă este necesară o inspecție pentru transport</t>
+  </si>
+  <si>
+    <t>Jei gabenamą krovinį reikia patikrinti</t>
+  </si>
+  <si>
+    <t>Ако има нужда от проверка на движението</t>
+  </si>
+  <si>
+    <t>Ha az árumozgatást ellenőrizni kell</t>
+  </si>
+  <si>
+    <t>Jeżeli przemieszczenie wymaga kontroli</t>
+  </si>
+  <si>
+    <t>Si el tránsito necesita inspección</t>
+  </si>
+  <si>
+    <t>Si le mouvement nécessite une inspection</t>
+  </si>
+  <si>
+    <t>Wenn für die Warenbeförderung eine Kontrolle erforderlich ist</t>
+  </si>
+  <si>
+    <t>Welsh</t>
+  </si>
+  <si>
+    <t>Os oes angen i’r symudiad hwn gael ei archwilio</t>
+  </si>
+  <si>
+    <t>start_page.before_you_start.inspection_needed</t>
+  </si>
   <si>
     <t>KEY</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>inspection_needed_import.bf_transit.heading</t>
-  </si>
-  <si>
-    <t>inspection_needed_export.bf_transit.heading</t>
-  </si>
-  <si>
-    <t>Für Ihre Transit-Kontrolle durch die Grenzbehörde (Border Force)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,47 +131,47 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helevetica"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +184,12 @@
         <bgColor rgb="FFBDBDBD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -121,21 +197,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -152,6 +213,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFCACACA"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCACACA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFCACACA"/>
@@ -162,56 +247,42 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{737C23FE-2062-7949-9733-88E9960A1E96}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{145767DE-5E71-4FDD-AAB0-DFA3AC73381F}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{0379D854-FC25-4F16-93FD-6B38214E7791}"/>
+    <cellStyle name="Normál 2" xfId="3" xr:uid="{66BDFD21-A3E8-4147-B676-F9F30F3B4BD9}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{2D952BDF-2BA3-48EA-9E89-B93B515F91F4}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,50 +593,424 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B2B6F4-4294-1B4B-ABAD-6BB5E6074097}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88F8323-D81A-7742-91D0-E5D4A31A9FBE}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="72.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="89.83203125" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="4"/>
+    <col min="1" max="1" width="43" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100" style="1" customWidth="1"/>
+    <col min="4" max="4" width="89.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="114.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="74.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="119.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="78.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="102" style="1" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="120.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="80.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="95" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
+    <row r="2" spans="1:13" ht="22">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:13">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="10"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D23464B46C9A6C438A9A63FA525492B5" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="816d63d098657adee5e1780dd4373ff3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78648aa0-189c-4913-b480-8f083842eefa" xmlns:ns3="252b28bd-d93f-4b99-825e-07b76ab2fd6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc6b77c161da750edc5730dfe65423ec" ns2:_="" ns3:_="">
+    <xsd:import namespace="78648aa0-189c-4913-b480-8f083842eefa"/>
+    <xsd:import namespace="252b28bd-d93f-4b99-825e-07b76ab2fd6b"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="78648aa0-189c-4913-b480-8f083842eefa" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a3ebb39f-d69b-4575-80f5-9912993956e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="252b28bd-d93f-4b99-825e-07b76ab2fd6b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f7f7e37a-fab3-43f2-9f32-1e0449a57439}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="252b28bd-d93f-4b99-825e-07b76ab2fd6b">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B41EF1-37C1-4B99-A8DD-7B54478B18A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4460EA2-5BBD-4FA9-A1BE-350942C106E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="78648aa0-189c-4913-b480-8f083842eefa"/>
+    <ds:schemaRef ds:uri="252b28bd-d93f-4b99-825e-07b76ab2fd6b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[RORO-5516][EL] fix - pr comment
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Croatian</t>
   </si>
   <si>
-    <t xml:space="preserve">inspection_needed_export.sad.heading</t>
+    <t xml:space="preserve">inspection_needed_export.mtp.heading</t>
   </si>
   <si>
     <t xml:space="preserve">For your Manual Transit Procedure endorsement</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Za vaše odobrenje neelektroničkog provoznog postupka</t>
   </si>
   <si>
-    <t xml:space="preserve">inspection_needed_import.sad.heading</t>
+    <t xml:space="preserve">inspection_needed_import.mtp.heading</t>
   </si>
 </sst>
 </file>
@@ -310,47 +310,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,7 +609,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="21" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -623,7 +623,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="78.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="102"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="79.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="120.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="120.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="80.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="11.5"/>

</xml_diff>

<commit_message>
[RORO-5850][JE] adds daera certex heading
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Translation" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Translation" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -61,46 +61,46 @@
     <t xml:space="preserve">Croatian</t>
   </si>
   <si>
-    <t xml:space="preserve">inspection_needed_export.mtp.heading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For your Manual Transit Procedure endorsement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar gyfer eich Gweithdrefn Cyffredinol Cludo â Llaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do indosu Twojej manualnej procedury tranzytowej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pentru aprobarea procedurii manuale pentru tranzit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dėl jūsų rankinės tranzito procedūros patvirtinimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">За потвърждение на вашия ръчен транзитен режим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A manuális árutovábbítási eljárás jóváhagyásához szükséges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para aprobación de su Procedimiento de Tránsito Manual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pour l’approbation de votre procédure de transit manuelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zur Bestätigung Ihres Manuellen Versandverfahrens „Manual Transit Procedure“</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pro vaše schválení manuálního postupu tranzitu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Za vaše odobrenje neelektroničkog provoznog postupka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inspection_needed_import.mtp.heading</t>
+    <t xml:space="preserve">inspection_needed_export.certex.heading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For your DAERA CERTEX inspection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ar gyfer eich archwiliad DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do Twojej kontroli DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentru inspecția dumneavoastră DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jūsų DAERA CERTEX patikrinimui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">За вашата CERTEX проверка от DAERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAERA CERTEX-ellenőrzés esetén</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para su inspección DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour votre inspection DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Für Ihre DAERA CERTEX-Prüfung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K prohlídce DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za inspekciju CERTEX DAERA-e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspection_needed_import.certex.heading</t>
   </si>
 </sst>
 </file>
@@ -111,10 +111,10 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -143,14 +143,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -158,7 +158,7 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -172,21 +172,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF172B4D"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Helvetica Neue"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -245,13 +233,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color theme="2"/>
+        <color rgb="FFE7E6E6"/>
       </left>
       <right style="thin">
-        <color theme="2"/>
+        <color rgb="FFE7E6E6"/>
       </right>
       <top style="thin">
-        <color theme="2"/>
+        <color rgb="FFE7E6E6"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -305,7 +293,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,18 +323,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,7 +392,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF172B4D"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -429,204 +405,32 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472c4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="21" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="100"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="89.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="114.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="74.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="74.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="119.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="78.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="102"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="79.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="120.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="120.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="80.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="11.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,104 +474,90 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
[RORO-5850][JE] fixes pr comments and bobby warning
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Croatian</t>
   </si>
   <si>
-    <t xml:space="preserve">inspection_needed_export.certex.heading</t>
+    <t xml:space="preserve">inspection_needed_export.daera_certex.heading</t>
   </si>
   <si>
     <t xml:space="preserve">For your DAERA CERTEX inspection</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Za inspekciju CERTEX DAERA-e</t>
   </si>
   <si>
-    <t xml:space="preserve">inspection_needed_import.certex.heading</t>
+    <t xml:space="preserve">inspection_needed_import.daera_certex.heading</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[RORO-5850][JE] Inspection UI: Display new Inspection location for DAERA Certex hold (#39)
* [RORO-5850][JE] adds daera certex heading

* [RORO-5850][JE] fixes pr comments and bobby warning
</commit_message>
<xml_diff>
--- a/test-resources/content_diff_file.xlsx
+++ b/test-resources/content_diff_file.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Translation" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Translation" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -61,46 +61,46 @@
     <t xml:space="preserve">Croatian</t>
   </si>
   <si>
-    <t xml:space="preserve">inspection_needed_export.mtp.heading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For your Manual Transit Procedure endorsement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar gyfer eich Gweithdrefn Cyffredinol Cludo â Llaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do indosu Twojej manualnej procedury tranzytowej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pentru aprobarea procedurii manuale pentru tranzit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dėl jūsų rankinės tranzito procedūros patvirtinimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">За потвърждение на вашия ръчен транзитен режим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A manuális árutovábbítási eljárás jóváhagyásához szükséges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para aprobación de su Procedimiento de Tránsito Manual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pour l’approbation de votre procédure de transit manuelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zur Bestätigung Ihres Manuellen Versandverfahrens „Manual Transit Procedure“</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pro vaše schválení manuálního postupu tranzitu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Za vaše odobrenje neelektroničkog provoznog postupka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inspection_needed_import.mtp.heading</t>
+    <t xml:space="preserve">inspection_needed_export.daera_certex.heading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For your DAERA CERTEX inspection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ar gyfer eich archwiliad DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do Twojej kontroli DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentru inspecția dumneavoastră DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jūsų DAERA CERTEX patikrinimui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">За вашата CERTEX проверка от DAERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAERA CERTEX-ellenőrzés esetén</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para su inspección DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour votre inspection DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Für Ihre DAERA CERTEX-Prüfung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K prohlídce DAERA CERTEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za inspekciju CERTEX DAERA-e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspection_needed_import.daera_certex.heading</t>
   </si>
 </sst>
 </file>
@@ -111,10 +111,10 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -143,14 +143,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -158,7 +158,7 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -172,21 +172,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF172B4D"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Helvetica Neue"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -245,13 +233,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color theme="2"/>
+        <color rgb="FFE7E6E6"/>
       </left>
       <right style="thin">
-        <color theme="2"/>
+        <color rgb="FFE7E6E6"/>
       </right>
       <top style="thin">
-        <color theme="2"/>
+        <color rgb="FFE7E6E6"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -305,7 +293,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,18 +323,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,7 +392,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF172B4D"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -429,204 +405,32 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472c4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="21" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="100"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="89.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="114.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="74.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="74.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="119.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="78.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="102"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="79.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="120.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="120.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="80.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="11.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,104 +474,90 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>